<commit_message>
add role matrix, update color scheme
</commit_message>
<xml_diff>
--- a/renergetic_ui/docs/roles.xlsx
+++ b/renergetic_ui/docs/roles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\ren\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\renergetic\renergetic_frontend\renergetic_ui\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
   <si>
     <t>Guest user (public): `guest`</t>
   </si>
@@ -134,12 +134,15 @@
 - 'notification'  -  user can or cannot get any notifications; could be removed (user-asset relation stored as connection_type in asset connections)
 - 'read'  -  can read data only if has connection with asser (asset_connection relation in RDBMS), managers can read everything</t>
   </si>
+  <si>
+    <t xml:space="preserve"> 'user_management'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,13 +160,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,9 +293,6 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -312,10 +305,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -327,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -353,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,62 +642,65 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.44140625" customWidth="1"/>
-    <col min="14" max="14" width="23.88671875" customWidth="1"/>
+    <col min="5" max="6" width="19" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" customWidth="1"/>
+    <col min="15" max="15" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L1" s="17" t="s">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-    </row>
-    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="25.8" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="1:16" ht="25.8" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -715,14 +714,15 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="L4" s="20" t="s">
+      <c r="K4" s="2"/>
+      <c r="M4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-    </row>
-    <row r="5" spans="1:15" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+    </row>
+    <row r="5" spans="1:16" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -734,19 +734,20 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="L5" s="19" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="M5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-    </row>
-    <row r="6" spans="1:15" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+    </row>
+    <row r="6" spans="1:16" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -759,16 +760,17 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+    </row>
+    <row r="7" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -779,22 +781,23 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-    </row>
-    <row r="8" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="K7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+    </row>
+    <row r="8" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -805,24 +808,27 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-    </row>
-    <row r="9" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="J8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -834,10 +840,10 @@
       <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
         <v>1</v>
       </c>
@@ -847,14 +853,19 @@
       <c r="I9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-    </row>
-    <row r="10" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="J9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -881,14 +892,19 @@
       <c r="I10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-    </row>
-    <row r="11" spans="1:15" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="J10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="1:16" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -915,29 +931,34 @@
       <c r="I11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L12" s="14" t="s">
+      <c r="J11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L12:O13"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="L5:O10"/>
-    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="M12:P13"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M5:P10"/>
+    <mergeCell ref="M4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -967,20 +988,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1011,12 +1032,12 @@
       <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1033,14 +1054,14 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="24"/>
+      <c r="N4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="26"/>
+      <c r="O4" s="25"/>
     </row>
     <row r="5" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1063,14 +1084,14 @@
       <c r="J5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="19" t="s">
+      <c r="M5" s="27"/>
+      <c r="N5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="19"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1097,10 +1118,10 @@
       <c r="J6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1131,10 +1152,10 @@
       <c r="J7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1167,10 +1188,10 @@
       <c r="J8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:15" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1205,18 +1226,18 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>